<commit_message>
test parameter freezing, inference on gpu
</commit_message>
<xml_diff>
--- a/model_comparisons.xlsx
+++ b/model_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Andrew\Code\RelationExtraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DEB502-C5F9-4662-9E81-422F978E1F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786102D6-7EE7-4CCC-B93B-254F84066C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{BD4C9907-59D3-4046-9EC5-60213A012C26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Untrained</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>~25 sec/iter on cpu</t>
+  </si>
+  <si>
+    <t>Frozen BERT, fine tuned classification head</t>
+  </si>
+  <si>
+    <t>~2 iter/sec, 375 iters</t>
+  </si>
+  <si>
+    <t>2.5 minutes</t>
+  </si>
+  <si>
+    <t>needs to relearn embeddings for entity labels?</t>
+  </si>
+  <si>
+    <t>Fine tuned embeddings and classification</t>
+  </si>
+  <si>
+    <t>4 minutes</t>
+  </si>
+  <si>
+    <t>~1.5 iter/sec, 375 iters</t>
   </si>
 </sst>
 </file>
@@ -403,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB413AE-A5DD-431E-8107-C7B4AB5CFD64}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +439,7 @@
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -426,12 +447,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -442,7 +463,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -457,6 +478,37 @@
       </c>
       <c r="E4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>0.2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added native torch training loop
</commit_message>
<xml_diff>
--- a/model_comparisons.xlsx
+++ b/model_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Andrew\Code\RelationExtraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786102D6-7EE7-4CCC-B93B-254F84066C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1596CD4-2077-450E-BF20-81D15B8ACE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{BD4C9907-59D3-4046-9EC5-60213A012C26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Untrained</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>~1.5 iter/sec, 375 iters</t>
+  </si>
+  <si>
+    <t>25 sec for 500 forward passes</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
+  <si>
+    <t>9s/iter, 38 iters</t>
+  </si>
+  <si>
+    <t>Low Resource? BERT (100 samples, 3 epochs)</t>
   </si>
 </sst>
 </file>
@@ -424,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB413AE-A5DD-431E-8107-C7B4AB5CFD64}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,9 +449,10 @@
     <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -447,12 +460,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -463,7 +476,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -480,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -497,7 +510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -509,6 +522,23 @@
       </c>
       <c r="D6" t="s">
         <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>